<commit_message>
toppings and decorations can be NULL for creation.  created urls and views for cookiecreation
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18520" yWindow="-14820" windowWidth="25600" windowHeight="15440" tabRatio="500"/>
+    <workbookView xWindow="9840" yWindow="-23960" windowWidth="26780" windowHeight="19680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>URL</t>
   </si>
@@ -149,6 +149,40 @@
   </si>
   <si>
     <t>json: message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">googlesign_in.  </t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>AllFlavorsView</t>
+  </si>
+  <si>
+    <t>AllCookieCuttersView</t>
+  </si>
+  <si>
+    <t>AllToppingsView</t>
+  </si>
+  <si>
+    <t>AllDecorationsView</t>
+  </si>
+  <si>
+    <t>get
+--auth header</t>
+  </si>
+  <si>
+    <t>json: all flavors</t>
+  </si>
+  <si>
+    <t>json: all cookie cutters</t>
+  </si>
+  <si>
+    <t>json: all toppings</t>
+  </si>
+  <si>
+    <t>json: all decorations</t>
   </si>
 </sst>
 </file>
@@ -466,21 +500,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,17 +535,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -526,8 +561,11 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -544,7 +582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -561,7 +599,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -578,7 +616,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
@@ -589,7 +627,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>34</v>
       </c>
@@ -606,34 +644,94 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created user_app and user_cookie_creation serializers. created view all and favorites views for user_cookie_creation
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>URL</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>empty</t>
-  </si>
-  <si>
-    <t>api/v1/userscookies/</t>
   </si>
   <si>
     <t>api/v1/cookiecreations/</t>
@@ -183,6 +180,39 @@
   </si>
   <si>
     <t>json: all decorations</t>
+  </si>
+  <si>
+    <t>all/</t>
+  </si>
+  <si>
+    <t>PublicCookieCreationsView</t>
+  </si>
+  <si>
+    <t>json: all previously bought cookie creations (where prev_purchased = t)</t>
+  </si>
+  <si>
+    <t>add/</t>
+  </si>
+  <si>
+    <t>favorites/</t>
+  </si>
+  <si>
+    <t>api/v1/mycookies/</t>
+  </si>
+  <si>
+    <t>AllUsersCreations</t>
+  </si>
+  <si>
+    <t>AllUsersFavorites</t>
+  </si>
+  <si>
+    <t>AddCreationToFavorites</t>
+  </si>
+  <si>
+    <t>json: all personal creations</t>
+  </si>
+  <si>
+    <t>json: all favorites</t>
   </si>
 </sst>
 </file>
@@ -503,15 +533,15 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -553,7 +583,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -562,7 +592,7 @@
         <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -573,7 +603,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -590,7 +620,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
@@ -607,10 +637,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
         <v>18</v>
@@ -618,10 +648,10 @@
     </row>
     <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -629,46 +659,101 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" t="s">
         <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
       </c>
       <c r="F9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>22</v>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
       <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
         <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>45</v>
       </c>
       <c r="F17" t="s">
         <v>18</v>
@@ -676,19 +761,19 @@
     </row>
     <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
         <v>18</v>
@@ -696,19 +781,19 @@
     </row>
     <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>18</v>
@@ -716,19 +801,19 @@
     </row>
     <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
added mailchimp_app and views
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="-23960" windowWidth="26780" windowHeight="19680" tabRatio="500"/>
+    <workbookView xWindow="16840" yWindow="-23840" windowWidth="28800" windowHeight="23380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>model url</t>
   </si>
   <si>
     <t>view name</t>
@@ -191,9 +188,6 @@
     <t>json: all previously bought cookie creations (where prev_purchased = t)</t>
   </si>
   <si>
-    <t>add/</t>
-  </si>
-  <si>
     <t>favorites/</t>
   </si>
   <si>
@@ -206,13 +200,69 @@
     <t>AllUsersFavorites</t>
   </si>
   <si>
-    <t>AddCreationToFavorites</t>
-  </si>
-  <si>
     <t>json: all personal creations</t>
   </si>
   <si>
     <t>json: all favorites</t>
+  </si>
+  <si>
+    <t>url.py name</t>
+  </si>
+  <si>
+    <t>adjustfavorites/&lt;int:cookie_creation_id&gt;/</t>
+  </si>
+  <si>
+    <t>AdjustFavorites</t>
+  </si>
+  <si>
+    <t>delete
+--auth header
+--json: empty</t>
+  </si>
+  <si>
+    <t>json: added cookie</t>
+  </si>
+  <si>
+    <t>api/v1/mailchimp/</t>
+  </si>
+  <si>
+    <t>test/</t>
+  </si>
+  <si>
+    <t>test_mailchimp</t>
+  </si>
+  <si>
+    <t>get
+--empty</t>
+  </si>
+  <si>
+    <t>json with okay status</t>
+  </si>
+  <si>
+    <t>subscribe/</t>
+  </si>
+  <si>
+    <t>Subscribe</t>
+  </si>
+  <si>
+    <t>unsubscribe/</t>
+  </si>
+  <si>
+    <t>Unsubscribe</t>
+  </si>
+  <si>
+    <t>post
+--json: email, first_name, last_name</t>
+  </si>
+  <si>
+    <t>post
+--json: email</t>
+  </si>
+  <si>
+    <t>deletemember/</t>
+  </si>
+  <si>
+    <t>DeleteMember</t>
   </si>
 </sst>
 </file>
@@ -530,15 +580,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
@@ -550,273 +601,368 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
-      </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
         <v>58</v>
       </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
       <c r="D19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
         <v>43</v>
       </c>
-      <c r="E19" t="s">
-        <v>45</v>
-      </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scary. i have only been pushing my back end for the last few hours, heres my front end
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22460" yWindow="-22600" windowWidth="24040" windowHeight="25980" tabRatio="500"/>
+    <workbookView xWindow="20520" yWindow="-28300" windowWidth="25980" windowHeight="28300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
   <si>
     <t>URL</t>
   </si>
@@ -117,9 +117,6 @@
 --json: empty</t>
   </si>
   <si>
-    <t>json: address</t>
-  </si>
-  <si>
     <t>get
 --auth header
 --json: empty</t>
@@ -271,6 +268,27 @@
     <t>post
 --auth header
 --json: prompt</t>
+  </si>
+  <si>
+    <t>json: display_name, email, address</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>all/remove/&lt;int:cookie_creation_id&gt;/</t>
+  </si>
+  <si>
+    <t>RemoveUserCreation</t>
+  </si>
+  <si>
+    <t>json: either removed from user or deleted</t>
+  </si>
+  <si>
+    <t>##adds cookie to users creations and makes it a favorite</t>
+  </si>
+  <si>
+    <t>##deletes cookie from database if not previously purchased, removes from user if previously purchased</t>
   </si>
 </sst>
 </file>
@@ -286,12 +304,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -306,11 +330,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,12 +629,12 @@
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -624,18 +649,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
@@ -651,8 +676,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
@@ -668,8 +693,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
@@ -685,7 +710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -693,167 +718,178 @@
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="D8" s="1" t="s">
+      <c r="E8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" t="s">
         <v>34</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D10" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D16" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" t="s">
-        <v>17</v>
-      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
         <v>36</v>
       </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
       <c r="D21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
         <v>41</v>
-      </c>
-      <c r="E21" t="s">
-        <v>43</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -861,19 +897,19 @@
     </row>
     <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -881,112 +917,132 @@
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C33" t="s">
         <v>61</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E33" t="s">
         <v>63</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="F31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+      <c r="C34" t="s">
         <v>65</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" t="s">
+        <v>34</v>
+      </c>
+      <c r="F34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="C35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
         <v>35</v>
       </c>
-      <c r="F32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="C40" t="s">
         <v>73</v>
       </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" t="s">
-        <v>35</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E40" t="s">
+        <v>34</v>
+      </c>
+      <c r="F40" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some css. created account page. excel crashed and lost views, had to redo
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20520" yWindow="-28300" windowWidth="25980" windowHeight="28300" tabRatio="500"/>
+    <workbookView xWindow="21700" yWindow="-28300" windowWidth="35380" windowHeight="28300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,84 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Robert Klingensmith</author>
+  </authors>
+  <commentList>
+    <comment ref="B7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Robert Klingensmith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+see put</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Robert Klingensmith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+when updating username it logs me out</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Robert Klingensmith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="91">
   <si>
     <t>URL</t>
   </si>
@@ -71,9 +147,6 @@
     <t>Info</t>
   </si>
   <si>
-    <t>json: token, client</t>
-  </si>
-  <si>
     <t>http</t>
   </si>
   <si>
@@ -102,10 +175,6 @@
   </si>
   <si>
     <t>api/v1/decorations/</t>
-  </si>
-  <si>
-    <t>post
---json: email, password</t>
   </si>
   <si>
     <t>post
@@ -127,9 +196,6 @@
 --json: address</t>
   </si>
   <si>
-    <t>json: display_name, address</t>
-  </si>
-  <si>
     <t>delete/</t>
   </si>
   <si>
@@ -192,12 +258,6 @@
   </si>
   <si>
     <t>AllUsersFavorites</t>
-  </si>
-  <si>
-    <t>json: all personal creations</t>
-  </si>
-  <si>
-    <t>json: all favorites</t>
   </si>
   <si>
     <t>url.py name</t>
@@ -270,32 +330,81 @@
 --json: prompt</t>
   </si>
   <si>
-    <t>json: display_name, email, address</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>all/remove/&lt;int:cookie_creation_id&gt;/</t>
-  </si>
-  <si>
-    <t>RemoveUserCreation</t>
-  </si>
-  <si>
-    <t>json: either removed from user or deleted</t>
-  </si>
-  <si>
-    <t>##adds cookie to users creations and makes it a favorite</t>
-  </si>
-  <si>
-    <t>##deletes cookie from database if not previously purchased, removes from user if previously purchased</t>
+    <t>addremove/&lt;int:cookie_creation_id&gt;/</t>
+  </si>
+  <si>
+    <t>post
+--json: email, password, display_name</t>
+  </si>
+  <si>
+    <t>json: user( from users display_name), email, address</t>
+  </si>
+  <si>
+    <t>json: display_name, address, password_updated(bool)</t>
+  </si>
+  <si>
+    <t>json: user( from users display_name), token</t>
+  </si>
+  <si>
+    <t>json: all creations in user_cookie_creation table, serialized</t>
+  </si>
+  <si>
+    <t>AddRemoveCreation</t>
+  </si>
+  <si>
+    <t>json: user cookie creation, serialized</t>
+  </si>
+  <si>
+    <t>json: all items in user_cookie_creation where is_favorite is true</t>
+  </si>
+  <si>
+    <t>##adds cookie to user_cookie_creation table if not there, then makes it favorite if it isn't</t>
+  </si>
+  <si>
+    <t>put
+--auth header
+--json: empty</t>
+  </si>
+  <si>
+    <t>##makes user_cookie_creation is_favorite equal to false. If it doesn’t exist or if it's already false returns error.</t>
+  </si>
+  <si>
+    <t>update/&lt;int:pk&gt;/</t>
+  </si>
+  <si>
+    <t>CreationPurchased</t>
+  </si>
+  <si>
+    <t>put:
+--auth header
+--json empty</t>
+  </si>
+  <si>
+    <t>json: new creation, serialized</t>
+  </si>
+  <si>
+    <t>create/</t>
+  </si>
+  <si>
+    <t>put:
+--auth header
+--json: name, description, flavor, cookie_cutter, topping (optional), decoration (optional), prev_purchased (optional), image</t>
+  </si>
+  <si>
+    <t>should this be 200, or 201?</t>
+  </si>
+  <si>
+    <t>should this be 200 or 204?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -303,8 +412,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,6 +434,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,12 +468,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,11 +757,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -646,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -659,7 +804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -667,13 +812,13 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -684,13 +829,13 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -701,195 +846,216 @@
         <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="D8" s="1" t="s">
-        <v>29</v>
+      <c r="D8" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
         <v>77</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
         <v>53</v>
       </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="D15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" t="s">
+    <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D17" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="F15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
+      <c r="B19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" t="s">
-        <v>41</v>
+        <v>88</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -897,156 +1063,186 @@
     </row>
     <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
+        <v>21</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
         <v>35</v>
       </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
       <c r="D27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
         <v>40</v>
       </c>
-      <c r="E27" t="s">
-        <v>44</v>
-      </c>
       <c r="F27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>59</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C36" t="s">
         <v>60</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="C37" t="s">
         <v>62</v>
       </c>
-      <c r="E33" t="s">
-        <v>63</v>
-      </c>
-      <c r="F33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+      <c r="D37" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E37" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
         <v>68</v>
       </c>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" t="s">
-        <v>71</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" t="s">
-        <v>34</v>
-      </c>
-      <c r="F36" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" t="s">
-        <v>17</v>
+      <c r="E42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
backend create cookie_creation. added to front end creations page. incorporated openai
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21700" yWindow="-28300" windowWidth="35380" windowHeight="28300" tabRatio="500"/>
+    <workbookView xWindow="23140" yWindow="-27040" windowWidth="35380" windowHeight="28300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,51 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+See Put</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Robert Klingensmith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+from AllCreationsPage can only add favorite, not remove</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Robert Klingensmith:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Once a user creates, they need to add it to their inventory</t>
         </r>
       </text>
     </comment>
@@ -103,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
   <si>
     <t>URL</t>
   </si>
@@ -319,9 +363,6 @@
     <t>DeleteMember</t>
   </si>
   <si>
-    <t>api/v1/openAI/</t>
-  </si>
-  <si>
     <t>ChatGPTQuery</t>
   </si>
   <si>
@@ -372,9 +413,6 @@
     <t>##makes user_cookie_creation is_favorite equal to false. If it doesn’t exist or if it's already false returns error.</t>
   </si>
   <si>
-    <t>update/&lt;int:pk&gt;/</t>
-  </si>
-  <si>
     <t>CreationPurchased</t>
   </si>
   <si>
@@ -389,25 +427,59 @@
     <t>create/</t>
   </si>
   <si>
-    <t>put:
+    <t>should this be 200, or 201?</t>
+  </si>
+  <si>
+    <t>should this be 200 or 204?</t>
+  </si>
+  <si>
+    <t>Front end Bad</t>
+  </si>
+  <si>
+    <t>All Good</t>
+  </si>
+  <si>
+    <t>Back end Bad</t>
+  </si>
+  <si>
+    <t>Back End Not Created</t>
+  </si>
+  <si>
+    <t>Both Ends Bad</t>
+  </si>
+  <si>
+    <t>Front End Not Created</t>
+  </si>
+  <si>
+    <t>Code for url.py name Column</t>
+  </si>
+  <si>
+    <t>purchased/&lt;int:pk&gt;/</t>
+  </si>
+  <si>
+    <t>post
 --auth header
 --json: name, description, flavor, cookie_cutter, topping (optional), decoration (optional), prev_purchased (optional), image</t>
   </si>
   <si>
-    <t>should this be 200, or 201?</t>
-  </si>
-  <si>
-    <t>should this be 200 or 204?</t>
+    <t>api/v1/openai/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -424,7 +496,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +527,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -468,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -476,11 +566,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -772,9 +865,10 @@
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -793,18 +887,27 @@
       <c r="F1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -812,16 +915,19 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="H4" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
@@ -832,13 +938,16 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="H5" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -854,9 +963,12 @@
       <c r="F6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+      <c r="H6" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
@@ -866,24 +978,27 @@
         <v>26</v>
       </c>
       <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="D8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
         <v>73</v>
       </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="D8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>74</v>
-      </c>
       <c r="F8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
@@ -900,12 +1015,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -919,32 +1034,32 @@
         <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
         <v>76</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" t="s">
-        <v>77</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>52</v>
@@ -956,7 +1071,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
@@ -967,14 +1082,14 @@
         <v>26</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B15" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C15" t="s">
@@ -990,12 +1105,12 @@
         <v>16</v>
       </c>
       <c r="G15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="D16" s="8" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="D16" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
@@ -1004,7 +1119,7 @@
         <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1031,17 +1146,17 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="F20" t="s">
         <v>16</v>
@@ -1049,13 +1164,13 @@
     </row>
     <row r="21" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -1178,7 +1293,7 @@
         <v>16</v>
       </c>
       <c r="G36" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1198,7 +1313,7 @@
         <v>16</v>
       </c>
       <c r="G37" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1218,21 +1333,21 @@
         <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
         <v>67</v>
       </c>
-      <c r="B42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="E42" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
sweetAlert for deleteUser. fixed update displayname, address logout issue. updated toDo list
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23140" yWindow="-27040" windowWidth="35380" windowHeight="28300" tabRatio="500"/>
+    <workbookView xWindow="24340" yWindow="-22820" windowWidth="35380" windowHeight="28300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,9 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-when updating username it logs me out</t>
+when updating username it logs me out.
+FIXED by just re-loading the page
+</t>
         </r>
       </text>
     </comment>
@@ -147,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
   <si>
     <t>URL</t>
   </si>
@@ -463,6 +465,9 @@
   </si>
   <si>
     <t>api/v1/openai/</t>
+  </si>
+  <si>
+    <t>CreateNewCreation</t>
   </si>
 </sst>
 </file>
@@ -496,7 +501,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +550,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -566,14 +577,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,7 +914,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="10" t="s">
         <v>93</v>
       </c>
     </row>
@@ -923,7 +934,7 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>88</v>
       </c>
     </row>
@@ -943,7 +954,7 @@
       <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>90</v>
       </c>
     </row>
@@ -963,12 +974,12 @@
       <c r="F6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
@@ -983,12 +994,12 @@
       <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E8" t="s">
@@ -1041,7 +1052,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C12" t="s">
@@ -1089,7 +1100,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C15" t="s">
@@ -1109,7 +1120,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="9" t="s">
         <v>80</v>
       </c>
       <c r="E16" t="s">
@@ -1146,7 +1157,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C20" t="s">
@@ -1163,8 +1174,11 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="144" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>96</v>
@@ -1260,7 +1274,7 @@
       <c r="A35" t="s">
         <v>54</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C35" t="s">
@@ -1277,7 +1291,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+      <c r="B36" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C36" t="s">
@@ -1297,7 +1311,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+      <c r="B37" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C37" t="s">
@@ -1317,7 +1331,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+      <c r="B38" s="10" t="s">
         <v>65</v>
       </c>
       <c r="C38" t="s">

</xml_diff>

<commit_message>
mailchimp. account page. signup page to meet mailchimps requirements
</commit_message>
<xml_diff>
--- a/Views.xlsx
+++ b/Views.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24340" yWindow="-22820" windowWidth="35380" windowHeight="28300" tabRatio="500"/>
+    <workbookView xWindow="24240" yWindow="-21520" windowWidth="35380" windowHeight="28300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="98">
   <si>
     <t>URL</t>
   </si>
@@ -355,10 +355,6 @@
 --json: email, first_name, last_name</t>
   </si>
   <si>
-    <t>post
---json: email</t>
-  </si>
-  <si>
     <t>deletemember/</t>
   </si>
   <si>
@@ -429,12 +425,6 @@
     <t>create/</t>
   </si>
   <si>
-    <t>should this be 200, or 201?</t>
-  </si>
-  <si>
-    <t>should this be 200 or 204?</t>
-  </si>
-  <si>
     <t>Front end Bad</t>
   </si>
   <si>
@@ -468,13 +458,21 @@
   </si>
   <si>
     <t>CreateNewCreation</t>
+  </si>
+  <si>
+    <t>put
+--json: email</t>
+  </si>
+  <si>
+    <t>delete
+--json: email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -500,25 +498,21 @@
       <color indexed="81"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -569,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,13 +572,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,23 +898,23 @@
         <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>89</v>
+      <c r="H2" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>93</v>
+      <c r="H3" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -926,16 +925,16 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>88</v>
+      <c r="H4" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -949,13 +948,13 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>90</v>
+      <c r="H5" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -974,8 +973,8 @@
       <c r="F6" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>91</v>
+      <c r="H6" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -989,21 +988,21 @@
         <v>26</v>
       </c>
       <c r="E7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="D8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
         <v>72</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="D8" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>73</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
@@ -1028,7 +1027,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -1045,24 +1044,24 @@
         <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="B12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="B12" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s">
-        <v>76</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -1070,7 +1069,7 @@
     </row>
     <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>52</v>
@@ -1093,7 +1092,7 @@
         <v>26</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
@@ -1116,12 +1115,12 @@
         <v>16</v>
       </c>
       <c r="G15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="D16" s="8" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="D16" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
@@ -1130,7 +1129,7 @@
         <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1140,7 +1139,7 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C19" t="s">
@@ -1157,34 +1156,34 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="144" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" t="s">
         <v>95</v>
       </c>
-      <c r="C20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="144" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -1194,7 +1193,7 @@
       <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C23" t="s">
@@ -1214,7 +1213,7 @@
       <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C25" t="s">
@@ -1234,7 +1233,7 @@
       <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C27" t="s">
@@ -1254,7 +1253,7 @@
       <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C29" t="s">
@@ -1270,28 +1269,28 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="B36" s="10" t="s">
+      <c r="F35" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C36" t="s">
@@ -1303,65 +1302,56 @@
       <c r="E36" t="s">
         <v>31</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="B37" s="10" t="s">
+      <c r="F36" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B37" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C37" t="s">
         <v>62</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
         <v>31</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="B38" s="10" t="s">
+      <c r="F37" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="B38" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
         <v>65</v>
       </c>
-      <c r="C38" t="s">
-        <v>66</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="E38" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="F38" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="E42" t="s">
         <v>31</v>

</xml_diff>